<commit_message>
Add more columns to Excel to add more options to bot
</commit_message>
<xml_diff>
--- a/Archivos.xlsx
+++ b/Archivos.xlsx
@@ -1,36 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABP\Desktop\Subir-Archivos-CF\Subir Archivos de Controladores Fiscales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\Subir-Archivos-CF\Subir Archivos de Controladores Fiscales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D0C655-82EB-45AD-81ED-2A571C712C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BCCEA5-30FB-4629-9BF2-1DF60DB2C457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Archivos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Archivo</t>
   </si>
   <si>
-    <t>Conrol</t>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Descargar Acuse</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Fila</t>
+  </si>
+  <si>
+    <t>Directorio de Guardado</t>
+  </si>
+  <si>
+    <t>Nombre de Guardado</t>
+  </si>
+  <si>
+    <t>ST</t>
   </si>
 </sst>
 </file>
@@ -363,23 +392,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <f>ROW()</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f>ROW()</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>ROW()</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <f>ROW()</f>
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D5" xr:uid="{570F3161-7961-4518-9150-7F18B9C576D9}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>